<commit_message>
included hours worked for bryan up to Dec 6
</commit_message>
<xml_diff>
--- a/documents/Burndown.xlsx
+++ b/documents/Burndown.xlsx
@@ -525,54 +525,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -590,30 +542,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -623,6 +554,75 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -867,11 +867,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97676672"/>
-        <c:axId val="97682560"/>
+        <c:axId val="69894528"/>
+        <c:axId val="69896064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97676672"/>
+        <c:axId val="69894528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,7 +880,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97682560"/>
+        <c:crossAx val="69896064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -888,7 +888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97682560"/>
+        <c:axId val="69896064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -899,7 +899,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97676672"/>
+        <c:crossAx val="69894528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1158,11 +1158,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99321728"/>
-        <c:axId val="99323264"/>
+        <c:axId val="69626496"/>
+        <c:axId val="69652864"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="99321728"/>
+        <c:axId val="69626496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1172,14 +1172,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99323264"/>
+        <c:crossAx val="69652864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="99323264"/>
+        <c:axId val="69652864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99321728"/>
+        <c:crossAx val="69626496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1243,93 +1243,75 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sp1'!$E$3:$P$3</c:f>
+              <c:f>'Sp2'!$E$3:$M$3</c:f>
               <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41939</c:v>
+                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>41975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41940</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41941</c:v>
+                  <c:v>41976</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41977</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41942</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41943</c:v>
+                  <c:v>41978</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41944</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41945</c:v>
+                  <c:v>41980</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41981</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41946</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41947</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41948</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41949</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41950</c:v>
+                  <c:v>41982</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sp1'!$D$48:$P$48</c:f>
+              <c:f>'Sp2'!$D$48:$M$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.25</c:v>
+                  <c:v>-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1347,93 +1329,75 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sp1'!$E$3:$P$3</c:f>
+              <c:f>'Sp2'!$E$3:$M$3</c:f>
               <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41939</c:v>
+                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>41975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41940</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41941</c:v>
+                  <c:v>41976</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41977</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41942</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41943</c:v>
+                  <c:v>41978</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41944</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41945</c:v>
+                  <c:v>41980</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41981</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41946</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41947</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41948</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="[$-409]d\-mmm;@">
-                  <c:v>41949</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41950</c:v>
+                  <c:v>41982</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sp1'!$D$49:$P$49</c:f>
+              <c:f>'Sp2'!$D$49:$M$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.53846153846154</c:v>
+                  <c:v>12.444444444444445</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.07692307692308</c:v>
+                  <c:v>10.888888888888889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.615384615384619</c:v>
+                  <c:v>9.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.153846153846157</c:v>
+                  <c:v>7.7777777777777786</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.692307692307695</c:v>
+                  <c:v>6.2222222222222232</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.230769230769234</c:v>
+                  <c:v>4.6666666666666679</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.7692307692307718</c:v>
+                  <c:v>3.1111111111111125</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.3076923076923102</c:v>
+                  <c:v>1.5555555555555569</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8461538461538485</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.3846153846153868</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.9230769230769251</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.4615384615384637</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1450,11 +1414,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97600640"/>
-        <c:axId val="97602176"/>
+        <c:axId val="69727360"/>
+        <c:axId val="69728896"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="97600640"/>
+        <c:axId val="69727360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,14 +1428,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97602176"/>
+        <c:crossAx val="69728896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="97602176"/>
+        <c:axId val="69728896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,7 +1446,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97600640"/>
+        <c:crossAx val="69727360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1916,13 +1880,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2232,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q49"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="Q38" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,22 +2213,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="46" t="s">
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="47"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="61"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
@@ -2379,10 +2343,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="72">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -2446,8 +2410,8 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="59"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="73"/>
       <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
@@ -2476,8 +2440,8 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="59"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2504,8 +2468,8 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="59"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="8" t="s">
         <v>18</v>
       </c>
@@ -2534,8 +2498,8 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
@@ -2597,8 +2561,8 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
@@ -2621,8 +2585,8 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="59"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
@@ -2651,8 +2615,8 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="59"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="8" t="s">
         <v>18</v>
       </c>
@@ -2675,8 +2639,8 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="73"/>
       <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
@@ -2738,8 +2702,8 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="73"/>
       <c r="C15" s="7" t="s">
         <v>16</v>
       </c>
@@ -2762,8 +2726,8 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
@@ -2786,8 +2750,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="60"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="8" t="s">
         <v>18</v>
       </c>
@@ -2814,8 +2778,8 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="58">
+      <c r="A18" s="63"/>
+      <c r="B18" s="72">
         <v>3</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -2879,8 +2843,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="59"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
@@ -2909,8 +2873,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="59"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
@@ -2933,8 +2897,8 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="60"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="8" t="s">
         <v>18</v>
       </c>
@@ -2957,10 +2921,10 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="51"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="9" t="s">
         <v>24</v>
       </c>
@@ -3022,8 +2986,8 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="7" t="s">
         <v>16</v>
       </c>
@@ -3046,8 +3010,8 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="52"/>
+      <c r="A24" s="63"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="7" t="s">
         <v>17</v>
       </c>
@@ -3074,8 +3038,8 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="8" t="s">
         <v>18</v>
       </c>
@@ -3098,10 +3062,10 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="54"/>
+      <c r="C26" s="68"/>
       <c r="D26" s="2">
         <f>SUM(D6,D10,D14,D18,D22)</f>
         <v>19</v>
@@ -3166,10 +3130,10 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="58">
+      <c r="B28" s="72">
         <v>2</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -3230,8 +3194,8 @@
       <c r="Q28" s="23"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="59"/>
+      <c r="A29" s="63"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="7" t="s">
         <v>16</v>
       </c>
@@ -3277,8 +3241,8 @@
       <c r="Q29" s="24"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="59"/>
+      <c r="A30" s="63"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="7" t="s">
         <v>17</v>
       </c>
@@ -3324,8 +3288,8 @@
       <c r="Q30" s="24"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
-      <c r="B31" s="59"/>
+      <c r="A31" s="63"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="8" t="s">
         <v>18</v>
       </c>
@@ -3371,8 +3335,8 @@
       <c r="Q31" s="24"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="59"/>
+      <c r="A32" s="63"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="9" t="s">
         <v>19</v>
       </c>
@@ -3431,8 +3395,8 @@
       <c r="Q32" s="23"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="59"/>
+      <c r="A33" s="63"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="7" t="s">
         <v>16</v>
       </c>
@@ -3452,8 +3416,8 @@
       <c r="Q33" s="24"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="59"/>
+      <c r="A34" s="63"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="7" t="s">
         <v>17</v>
       </c>
@@ -3499,8 +3463,8 @@
       <c r="Q34" s="24"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="59"/>
+      <c r="A35" s="63"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="8" t="s">
         <v>18</v>
       </c>
@@ -3520,8 +3484,8 @@
       <c r="Q35" s="24"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
-      <c r="B36" s="59"/>
+      <c r="A36" s="63"/>
+      <c r="B36" s="73"/>
       <c r="C36" s="9" t="s">
         <v>20</v>
       </c>
@@ -3580,8 +3544,8 @@
       <c r="Q36" s="23"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="49"/>
-      <c r="B37" s="59"/>
+      <c r="A37" s="63"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="7" t="s">
         <v>16</v>
       </c>
@@ -3601,8 +3565,8 @@
       <c r="Q37" s="24"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="49"/>
-      <c r="B38" s="59"/>
+      <c r="A38" s="63"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="7" t="s">
         <v>17</v>
       </c>
@@ -3622,8 +3586,8 @@
       <c r="Q38" s="24"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="49"/>
-      <c r="B39" s="60"/>
+      <c r="A39" s="63"/>
+      <c r="B39" s="74"/>
       <c r="C39" s="8" t="s">
         <v>18</v>
       </c>
@@ -3669,8 +3633,8 @@
       <c r="Q39" s="24"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
-      <c r="B40" s="58">
+      <c r="A40" s="63"/>
+      <c r="B40" s="72">
         <v>3</v>
       </c>
       <c r="C40" s="9" t="s">
@@ -3731,8 +3695,8 @@
       <c r="Q40" s="23"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
-      <c r="B41" s="59"/>
+      <c r="A41" s="63"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="7" t="s">
         <v>16</v>
       </c>
@@ -3778,8 +3742,8 @@
       <c r="Q41" s="24"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
-      <c r="B42" s="59"/>
+      <c r="A42" s="63"/>
+      <c r="B42" s="73"/>
       <c r="C42" s="7" t="s">
         <v>17</v>
       </c>
@@ -3799,8 +3763,8 @@
       <c r="Q42" s="24"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
-      <c r="B43" s="60"/>
+      <c r="A43" s="64"/>
+      <c r="B43" s="74"/>
       <c r="C43" s="8" t="s">
         <v>18</v>
       </c>
@@ -3820,10 +3784,10 @@
       <c r="Q43" s="24"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="48" t="s">
+      <c r="A44" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="51"/>
+      <c r="B44" s="65"/>
       <c r="C44" s="9" t="s">
         <v>24</v>
       </c>
@@ -3882,8 +3846,8 @@
       <c r="Q44" s="23"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
-      <c r="B45" s="52"/>
+      <c r="A45" s="63"/>
+      <c r="B45" s="66"/>
       <c r="C45" s="7" t="s">
         <v>16</v>
       </c>
@@ -3903,8 +3867,8 @@
       <c r="Q45" s="24"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="49"/>
-      <c r="B46" s="52"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="66"/>
       <c r="C46" s="7" t="s">
         <v>17</v>
       </c>
@@ -3950,8 +3914,8 @@
       <c r="Q46" s="24"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
-      <c r="B47" s="53"/>
+      <c r="A47" s="64"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="8" t="s">
         <v>18</v>
       </c>
@@ -3971,10 +3935,10 @@
       <c r="Q47" s="24"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="54" t="s">
+      <c r="B48" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="54"/>
+      <c r="C48" s="68"/>
       <c r="D48" s="2">
         <f>SUM(D28,D32,D36,D40,D44)</f>
         <v>19</v>
@@ -4112,8 +4076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4130,19 +4094,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="55" t="s">
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="57"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="71"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
@@ -4209,33 +4173,33 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="75" t="s">
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="54" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="68">
+      <c r="B6" s="75">
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -4282,14 +4246,14 @@
         <v>0</v>
       </c>
       <c r="N6" s="14">
-        <f>SUM(E6:M6)</f>
+        <f t="shared" ref="N6:N26" si="1">SUM(E6:M6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="61" t="s">
+      <c r="A7" s="63"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="45" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="24"/>
@@ -4303,14 +4267,14 @@
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
       <c r="N7" s="28">
-        <f>SUM(E7:M7)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="61" t="s">
+      <c r="A8" s="63"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="24">
@@ -4326,14 +4290,14 @@
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
       <c r="N8" s="28">
-        <f>SUM(E8:M8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="62" t="s">
+      <c r="A9" s="63"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="26"/>
@@ -4347,16 +4311,16 @@
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
       <c r="N9" s="30">
-        <f>SUM(E9:M9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="71" t="s">
+      <c r="A10" s="63"/>
+      <c r="B10" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="47" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="10">
@@ -4364,50 +4328,50 @@
         <v>1</v>
       </c>
       <c r="E10" s="16">
-        <f t="shared" ref="E10:M10" si="1">SUM(E11:E13)</f>
+        <f t="shared" ref="E10:M10" si="2">SUM(E11:E13)</f>
         <v>0</v>
       </c>
       <c r="F10" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="14">
-        <f>SUM(E10:M10)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="61" t="s">
+      <c r="A11" s="63"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="24"/>
@@ -4421,14 +4385,14 @@
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
       <c r="N11" s="28">
-        <f>SUM(E11:M11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="61" t="s">
+      <c r="A12" s="63"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="24"/>
@@ -4442,14 +4406,14 @@
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
       <c r="N12" s="28">
-        <f>SUM(E12:M12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="62" t="s">
+      <c r="A13" s="63"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="26">
@@ -4465,14 +4429,14 @@
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
       <c r="N13" s="30">
-        <f>SUM(E13:M13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="73" t="s">
+      <c r="A14" s="63"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="52" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="10">
@@ -4480,50 +4444,50 @@
         <v>6</v>
       </c>
       <c r="E14" s="16">
-        <f t="shared" ref="E14:M14" si="2">SUM(E15:E17)</f>
+        <f t="shared" ref="E14:M14" si="3">SUM(E15:E17)</f>
         <v>0</v>
       </c>
       <c r="F14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N14" s="14">
-        <f>SUM(E14:M14)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="61" t="s">
+      <c r="A15" s="63"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="45" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="24">
@@ -4543,14 +4507,14 @@
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
       <c r="N15" s="28">
-        <f>SUM(E15:M15)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="61" t="s">
+      <c r="A16" s="63"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="24">
@@ -4566,14 +4530,14 @@
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
       <c r="N16" s="28">
-        <f>SUM(E16:M16)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="61" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="45" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="24"/>
@@ -4587,15 +4551,15 @@
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
       <c r="N17" s="28">
-        <f>SUM(E17:M17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="58"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="10" t="s">
         <v>34</v>
       </c>
@@ -4604,50 +4568,50 @@
         <v>4</v>
       </c>
       <c r="E18" s="16">
-        <f t="shared" ref="E18:M18" si="3">SUM(E19:E21)</f>
+        <f t="shared" ref="E18:M18" si="4">SUM(E19:E21)</f>
         <v>0</v>
       </c>
       <c r="F18" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G18" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H18" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I18" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J18" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K18" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L18" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M18" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N18" s="14">
-        <f>SUM(E18:M18)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="61" t="s">
+      <c r="A19" s="63"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="45" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="24">
@@ -4665,14 +4629,14 @@
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
       <c r="N19" s="28">
-        <f>SUM(E19:M19)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="61" t="s">
+      <c r="A20" s="63"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="24">
@@ -4688,14 +4652,14 @@
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
       <c r="N20" s="28">
-        <f>SUM(E20:M20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="62" t="s">
+      <c r="A21" s="63"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="26"/>
@@ -4709,65 +4673,65 @@
       <c r="L21" s="29"/>
       <c r="M21" s="29"/>
       <c r="N21" s="30">
-        <f>SUM(E21:M21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="65" t="s">
+      <c r="A22" s="63"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="49">
         <f>SUM(D23:D25)</f>
         <v>1</v>
       </c>
-      <c r="E22" s="66">
-        <f t="shared" ref="E22:M22" si="4">SUM(E23:E25)</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="66">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="66">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="66">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="66">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="66">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="66">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="66">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="66">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="67">
-        <f>SUM(E22:M22)</f>
+      <c r="E22" s="50">
+        <f t="shared" ref="E22:M22" si="5">SUM(E23:E25)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="51">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="76"/>
-      <c r="C23" s="61" t="s">
+      <c r="A23" s="63"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="45" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="19"/>
@@ -4781,14 +4745,14 @@
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
       <c r="N23" s="28">
-        <f>SUM(E23:M23)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="61" t="s">
+      <c r="A24" s="63"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="25"/>
@@ -4802,14 +4766,14 @@
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
       <c r="N24" s="28">
-        <f>SUM(E24:M24)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="77"/>
-      <c r="C25" s="62" t="s">
+      <c r="A25" s="64"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="26">
@@ -4825,57 +4789,57 @@
       <c r="L25" s="29"/>
       <c r="M25" s="29"/>
       <c r="N25" s="30">
-        <f>SUM(E25:M25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="54"/>
+      <c r="C26" s="68"/>
       <c r="D26" s="2">
         <f>SUM(D6,D10,D14,D18,D22)</f>
         <v>14</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" ref="E26:M26" si="5">SUM(E6,E10,E14,E18,E22)</f>
+        <f t="shared" ref="E26:M26" si="6">SUM(E6,E10,E14,E18,E22)</f>
         <v>0</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N26" s="23">
-        <f>SUM(E26:M26)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -4886,10 +4850,10 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="68">
+      <c r="B28" s="75">
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -4900,51 +4864,51 @@
         <v>2</v>
       </c>
       <c r="E28" s="16">
-        <f t="shared" ref="E28:M28" si="6">SUM(E29:E31)</f>
+        <f t="shared" ref="E28:M28" si="7">SUM(E29:E31)</f>
         <v>0</v>
       </c>
       <c r="F28" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G28" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H28" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I28" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J28" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K28" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L28" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M28" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N28" s="23"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="61" t="s">
+      <c r="A29" s="63"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="80">
-        <f t="shared" ref="D29:D47" si="7">D7</f>
+      <c r="D29" s="57">
+        <f t="shared" ref="D29:D47" si="8">D7</f>
         <v>0</v>
       </c>
       <c r="E29" s="31"/>
@@ -4959,13 +4923,13 @@
       <c r="N29" s="24"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="61" t="s">
+      <c r="A30" s="63"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="80">
-        <f t="shared" si="7"/>
+      <c r="D30" s="57">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="E30" s="31"/>
@@ -4980,13 +4944,13 @@
       <c r="N30" s="24"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="62" t="s">
+      <c r="A31" s="63"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="81">
-        <f t="shared" si="7"/>
+      <c r="D31" s="58">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E31" s="31"/>
@@ -5001,70 +4965,80 @@
       <c r="N31" s="24"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="71" t="s">
+      <c r="A32" s="63"/>
+      <c r="B32" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="63" t="s">
+      <c r="C32" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="79">
-        <f t="shared" si="7"/>
+      <c r="D32" s="56">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="E32" s="16">
-        <f t="shared" ref="E32:M32" si="8">SUM(E33:E35)</f>
+        <f t="shared" ref="E32:M32" si="9">SUM(E33:E35)</f>
         <v>0</v>
       </c>
       <c r="F32" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="16">
+        <f t="shared" si="9"/>
+        <v>-0.5</v>
+      </c>
+      <c r="J32" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="23"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="63"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="57">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G32" s="16">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="16">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="16">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="16">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K32" s="16">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L32" s="16">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="16">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="23"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="80">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
+      <c r="E33" s="31">
+        <v>0</v>
+      </c>
+      <c r="F33" s="31">
+        <v>0</v>
+      </c>
+      <c r="G33" s="32">
+        <v>0</v>
+      </c>
+      <c r="H33" s="32">
+        <v>0</v>
+      </c>
+      <c r="I33" s="32">
+        <v>-0.5</v>
+      </c>
       <c r="J33" s="32"/>
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
@@ -5072,13 +5046,13 @@
       <c r="N33" s="24"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="61" t="s">
+      <c r="A34" s="63"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="80">
-        <f t="shared" si="7"/>
+      <c r="D34" s="57">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E34" s="31"/>
@@ -5093,13 +5067,13 @@
       <c r="N34" s="24"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="62" t="s">
+      <c r="A35" s="63"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="81">
-        <f t="shared" si="7"/>
+      <c r="D35" s="58">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="E35" s="33"/>
@@ -5114,61 +5088,61 @@
       <c r="N35" s="24"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
-      <c r="B36" s="72"/>
-      <c r="C36" s="73" t="s">
+      <c r="A36" s="63"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="79">
-        <f t="shared" si="7"/>
+      <c r="D36" s="56">
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="E36" s="16">
-        <f t="shared" ref="E36:M36" si="9">SUM(E37:E39)</f>
+        <f t="shared" ref="E36:M36" si="10">SUM(E37:E39)</f>
         <v>0</v>
       </c>
       <c r="F36" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G36" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H36" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I36" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J36" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K36" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L36" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M36" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N36" s="23"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="49"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="61" t="s">
+      <c r="A37" s="63"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="80">
-        <f t="shared" si="7"/>
+      <c r="D37" s="57">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="E37" s="31"/>
@@ -5183,13 +5157,13 @@
       <c r="N37" s="24"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="49"/>
-      <c r="B38" s="72"/>
-      <c r="C38" s="61" t="s">
+      <c r="A38" s="63"/>
+      <c r="B38" s="79"/>
+      <c r="C38" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="80">
-        <f t="shared" si="7"/>
+      <c r="D38" s="57">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="E38" s="31"/>
@@ -5204,13 +5178,13 @@
       <c r="N38" s="24"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="49"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="61" t="s">
+      <c r="A39" s="63"/>
+      <c r="B39" s="79"/>
+      <c r="C39" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="81">
-        <f t="shared" si="7"/>
+      <c r="D39" s="58">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E39" s="33"/>
@@ -5225,70 +5199,80 @@
       <c r="N39" s="24"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="58"/>
+      <c r="B40" s="72"/>
       <c r="C40" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="79">
-        <f t="shared" si="7"/>
+      <c r="D40" s="56">
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="E40" s="16">
-        <f t="shared" ref="E40:M40" si="10">SUM(E41:E43)</f>
-        <v>0</v>
+        <f t="shared" ref="E40:M40" si="11">SUM(E41:E43)</f>
+        <v>2</v>
       </c>
       <c r="F40" s="16">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>2</v>
       </c>
       <c r="G40" s="16">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>2</v>
       </c>
       <c r="H40" s="16">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>2</v>
       </c>
       <c r="I40" s="16">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>-3.5</v>
       </c>
       <c r="J40" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K40" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L40" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M40" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N40" s="23"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="61" t="s">
+      <c r="A41" s="63"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="80">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
+      <c r="D41" s="57">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E41" s="31">
+        <v>2</v>
+      </c>
+      <c r="F41" s="31">
+        <v>2</v>
+      </c>
+      <c r="G41" s="31">
+        <v>2</v>
+      </c>
+      <c r="H41" s="31">
+        <v>2</v>
+      </c>
+      <c r="I41" s="31">
+        <v>-3.5</v>
+      </c>
       <c r="J41" s="31"/>
       <c r="K41" s="31"/>
       <c r="L41" s="31"/>
@@ -5296,13 +5280,13 @@
       <c r="N41" s="24"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
-      <c r="B42" s="59"/>
-      <c r="C42" s="61" t="s">
+      <c r="A42" s="63"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="80">
-        <f t="shared" si="7"/>
+      <c r="D42" s="57">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="E42" s="31"/>
@@ -5317,13 +5301,13 @@
       <c r="N42" s="24"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="62" t="s">
+      <c r="A43" s="63"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="81">
-        <f t="shared" si="7"/>
+      <c r="D43" s="58">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E43" s="33"/>
@@ -5338,61 +5322,61 @@
       <c r="N43" s="24"/>
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49"/>
-      <c r="B44" s="76"/>
-      <c r="C44" s="65" t="s">
+      <c r="A44" s="63"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="79">
-        <f t="shared" si="7"/>
+      <c r="D44" s="56">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="E44" s="21">
-        <f t="shared" ref="E44:M44" si="11">SUM(E45:E47)</f>
+        <f t="shared" ref="E44:M44" si="12">SUM(E45:E47)</f>
         <v>0</v>
       </c>
       <c r="F44" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G44" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H44" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I44" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J44" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K44" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L44" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M44" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N44" s="23"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
-      <c r="B45" s="76"/>
-      <c r="C45" s="61" t="s">
+      <c r="A45" s="63"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="80">
-        <f t="shared" si="7"/>
+      <c r="D45" s="57">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E45" s="31"/>
@@ -5407,13 +5391,13 @@
       <c r="N45" s="24"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="49"/>
-      <c r="B46" s="76"/>
-      <c r="C46" s="61" t="s">
+      <c r="A46" s="63"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="80">
-        <f t="shared" si="7"/>
+      <c r="D46" s="57">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E46" s="31"/>
@@ -5428,13 +5412,13 @@
       <c r="N46" s="24"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="62" t="s">
+      <c r="A47" s="64"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="81">
-        <f t="shared" si="7"/>
+      <c r="D47" s="58">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="E47" s="33"/>
@@ -5449,48 +5433,48 @@
       <c r="N47" s="24"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="54" t="s">
+      <c r="B48" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="54"/>
+      <c r="C48" s="68"/>
       <c r="D48" s="2">
         <f>SUM(D28,D32,D36,D40,D44)</f>
         <v>14</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" ref="E48:M48" si="12">SUM(E28,E32,E36,E40,E44)</f>
-        <v>0</v>
+        <f t="shared" ref="E48:M48" si="13">SUM(E28,E32,E36,E40,E44)</f>
+        <v>2</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>2</v>
       </c>
       <c r="G48" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>2</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>2</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-4</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K48" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L48" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M48" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N48" s="23"/>
@@ -5501,44 +5485,50 @@
         <v>14</v>
       </c>
       <c r="E49">
-        <f xml:space="preserve"> D49 - ($D$49/COUNT($D$4:$M$4))</f>
+        <f t="shared" ref="E49:M49" si="14" xml:space="preserve"> D49 - ($D$49/COUNT($D$4:$M$4))</f>
         <v>12.444444444444445</v>
       </c>
       <c r="F49">
-        <f xml:space="preserve"> E49 - ($D$49/COUNT($D$4:$M$4))</f>
+        <f t="shared" si="14"/>
         <v>10.888888888888889</v>
       </c>
       <c r="G49">
-        <f xml:space="preserve"> F49 - ($D$49/COUNT($D$4:$M$4))</f>
+        <f t="shared" si="14"/>
         <v>9.3333333333333339</v>
       </c>
       <c r="H49">
-        <f xml:space="preserve"> G49 - ($D$49/COUNT($D$4:$M$4))</f>
+        <f t="shared" si="14"/>
         <v>7.7777777777777786</v>
       </c>
       <c r="I49">
-        <f xml:space="preserve"> H49 - ($D$49/COUNT($D$4:$M$4))</f>
+        <f t="shared" si="14"/>
         <v>6.2222222222222232</v>
       </c>
       <c r="J49">
-        <f xml:space="preserve"> I49 - ($D$49/COUNT($D$4:$M$4))</f>
+        <f t="shared" si="14"/>
         <v>4.6666666666666679</v>
       </c>
       <c r="K49">
-        <f xml:space="preserve"> J49 - ($D$49/COUNT($D$4:$M$4))</f>
+        <f t="shared" si="14"/>
         <v>3.1111111111111125</v>
       </c>
       <c r="L49">
-        <f xml:space="preserve"> K49 - ($D$49/COUNT($D$4:$M$4))</f>
+        <f t="shared" si="14"/>
         <v>1.5555555555555569</v>
       </c>
       <c r="M49">
-        <f xml:space="preserve"> L49 - ($D$49/COUNT($D$4:$M$4))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A28:A39"/>
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A6:A17"/>
+    <mergeCell ref="A18:A25"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -5549,12 +5539,6 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A28:A39"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A6:A17"/>
-    <mergeCell ref="A18:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated sprint documents with bryan's times
</commit_message>
<xml_diff>
--- a/documents/Burndown.xlsx
+++ b/documents/Burndown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Product Burndown" sheetId="1" r:id="rId1"/>
@@ -603,6 +603,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -617,12 +623,6 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -867,11 +867,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69894528"/>
-        <c:axId val="69896064"/>
+        <c:axId val="88637824"/>
+        <c:axId val="88639360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69894528"/>
+        <c:axId val="88637824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,7 +880,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69896064"/>
+        <c:crossAx val="88639360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -888,7 +888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69896064"/>
+        <c:axId val="88639360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -899,13 +899,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69894528"/>
+        <c:crossAx val="88637824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1158,11 +1159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69626496"/>
-        <c:axId val="69652864"/>
+        <c:axId val="88959616"/>
+        <c:axId val="88985984"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="69626496"/>
+        <c:axId val="88959616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1172,14 +1173,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69652864"/>
+        <c:crossAx val="88985984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="69652864"/>
+        <c:axId val="88985984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,14 +1191,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69626496"/>
+        <c:crossAx val="88959616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1287,31 +1287,31 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-4.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>-4.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>-4.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,11 +1414,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69727360"/>
-        <c:axId val="69728896"/>
+        <c:axId val="90629248"/>
+        <c:axId val="90630784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="69727360"/>
+        <c:axId val="90629248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,14 +1428,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69728896"/>
+        <c:crossAx val="90630784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="69728896"/>
+        <c:axId val="90630784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +1446,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69727360"/>
+        <c:crossAx val="90629248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1864,7 +1864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -4076,8 +4076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4199,7 +4199,7 @@
       <c r="A6" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="75">
+      <c r="B6" s="77">
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -4252,7 +4252,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="63"/>
-      <c r="B7" s="76"/>
+      <c r="B7" s="78"/>
       <c r="C7" s="45" t="s">
         <v>16</v>
       </c>
@@ -4273,7 +4273,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="63"/>
-      <c r="B8" s="76"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
@@ -4296,7 +4296,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="63"/>
-      <c r="B9" s="77"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -4317,7 +4317,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="63"/>
-      <c r="B10" s="78" t="s">
+      <c r="B10" s="80" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -4370,7 +4370,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="63"/>
-      <c r="B11" s="79"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
@@ -4391,7 +4391,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="63"/>
-      <c r="B12" s="79"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
@@ -4412,7 +4412,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="63"/>
-      <c r="B13" s="79"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -4435,7 +4435,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="63"/>
-      <c r="B14" s="79"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="52" t="s">
         <v>33</v>
       </c>
@@ -4486,7 +4486,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="63"/>
-      <c r="B15" s="79"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="45" t="s">
         <v>16</v>
       </c>
@@ -4513,7 +4513,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="63"/>
-      <c r="B16" s="79"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="63"/>
-      <c r="B17" s="79"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="45" t="s">
         <v>18</v>
       </c>
@@ -4679,7 +4679,7 @@
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="63"/>
-      <c r="B22" s="80"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="49" t="s">
         <v>31</v>
       </c>
@@ -4730,7 +4730,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="63"/>
-      <c r="B23" s="80"/>
+      <c r="B23" s="75"/>
       <c r="C23" s="45" t="s">
         <v>16</v>
       </c>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="63"/>
-      <c r="B24" s="80"/>
+      <c r="B24" s="75"/>
       <c r="C24" s="45" t="s">
         <v>17</v>
       </c>
@@ -4772,7 +4772,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="64"/>
-      <c r="B25" s="81"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -4853,7 +4853,7 @@
       <c r="A28" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="75">
+      <c r="B28" s="77">
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -4903,7 +4903,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="63"/>
-      <c r="B29" s="76"/>
+      <c r="B29" s="78"/>
       <c r="C29" s="45" t="s">
         <v>16</v>
       </c>
@@ -4924,7 +4924,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="63"/>
-      <c r="B30" s="76"/>
+      <c r="B30" s="78"/>
       <c r="C30" s="45" t="s">
         <v>17</v>
       </c>
@@ -4945,7 +4945,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="63"/>
-      <c r="B31" s="77"/>
+      <c r="B31" s="79"/>
       <c r="C31" s="46" t="s">
         <v>18</v>
       </c>
@@ -4966,7 +4966,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="63"/>
-      <c r="B32" s="78" t="s">
+      <c r="B32" s="80" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="47" t="s">
@@ -4998,25 +4998,25 @@
       </c>
       <c r="J32" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K32" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L32" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M32" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N32" s="23"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="63"/>
-      <c r="B33" s="79"/>
+      <c r="B33" s="81"/>
       <c r="C33" s="45" t="s">
         <v>16</v>
       </c>
@@ -5039,15 +5039,23 @@
       <c r="I33" s="32">
         <v>-0.5</v>
       </c>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
+      <c r="J33" s="32">
+        <v>-1</v>
+      </c>
+      <c r="K33" s="32">
+        <v>-1</v>
+      </c>
+      <c r="L33" s="32">
+        <v>-1</v>
+      </c>
+      <c r="M33" s="32">
+        <v>-1</v>
+      </c>
       <c r="N33" s="24"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="63"/>
-      <c r="B34" s="79"/>
+      <c r="B34" s="81"/>
       <c r="C34" s="45" t="s">
         <v>17</v>
       </c>
@@ -5068,7 +5076,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="63"/>
-      <c r="B35" s="79"/>
+      <c r="B35" s="81"/>
       <c r="C35" s="46" t="s">
         <v>18</v>
       </c>
@@ -5089,7 +5097,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="63"/>
-      <c r="B36" s="79"/>
+      <c r="B36" s="81"/>
       <c r="C36" s="52" t="s">
         <v>33</v>
       </c>
@@ -5099,27 +5107,27 @@
       </c>
       <c r="E36" s="16">
         <f t="shared" ref="E36:M36" si="10">SUM(E37:E39)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F36" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G36" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I36" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J36" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K36" s="16">
         <f t="shared" si="10"/>
@@ -5137,7 +5145,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="63"/>
-      <c r="B37" s="79"/>
+      <c r="B37" s="81"/>
       <c r="C37" s="45" t="s">
         <v>16</v>
       </c>
@@ -5145,12 +5153,24 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
+      <c r="E37" s="31">
+        <v>3</v>
+      </c>
+      <c r="F37" s="31">
+        <v>3</v>
+      </c>
+      <c r="G37" s="31">
+        <v>3</v>
+      </c>
+      <c r="H37" s="31">
+        <v>3</v>
+      </c>
+      <c r="I37" s="31">
+        <v>3</v>
+      </c>
+      <c r="J37" s="32">
+        <v>1.5</v>
+      </c>
       <c r="K37" s="32"/>
       <c r="L37" s="32"/>
       <c r="M37" s="32"/>
@@ -5158,7 +5178,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="63"/>
-      <c r="B38" s="79"/>
+      <c r="B38" s="81"/>
       <c r="C38" s="45" t="s">
         <v>17</v>
       </c>
@@ -5179,7 +5199,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="63"/>
-      <c r="B39" s="79"/>
+      <c r="B39" s="81"/>
       <c r="C39" s="45" t="s">
         <v>18</v>
       </c>
@@ -5232,19 +5252,19 @@
       </c>
       <c r="J40" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-3.5</v>
       </c>
       <c r="K40" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-3.5</v>
       </c>
       <c r="L40" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-3.5</v>
       </c>
       <c r="M40" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-3.5</v>
       </c>
       <c r="N40" s="23"/>
     </row>
@@ -5273,10 +5293,18 @@
       <c r="I41" s="31">
         <v>-3.5</v>
       </c>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
+      <c r="J41" s="31">
+        <v>-3.5</v>
+      </c>
+      <c r="K41" s="31">
+        <v>-3.5</v>
+      </c>
+      <c r="L41" s="31">
+        <v>-3.5</v>
+      </c>
+      <c r="M41" s="31">
+        <v>-3.5</v>
+      </c>
       <c r="N41" s="24"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -5323,7 +5351,7 @@
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="63"/>
-      <c r="B44" s="80"/>
+      <c r="B44" s="75"/>
       <c r="C44" s="49" t="s">
         <v>31</v>
       </c>
@@ -5371,7 +5399,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="63"/>
-      <c r="B45" s="80"/>
+      <c r="B45" s="75"/>
       <c r="C45" s="45" t="s">
         <v>16</v>
       </c>
@@ -5392,7 +5420,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="63"/>
-      <c r="B46" s="80"/>
+      <c r="B46" s="75"/>
       <c r="C46" s="45" t="s">
         <v>17</v>
       </c>
@@ -5413,7 +5441,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="64"/>
-      <c r="B47" s="81"/>
+      <c r="B47" s="76"/>
       <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
@@ -5443,39 +5471,39 @@
       </c>
       <c r="E48" s="2">
         <f t="shared" ref="E48:M48" si="13">SUM(E28,E32,E36,E40,E44)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F48" s="2">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" si="13"/>
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="K48" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-4.5</v>
       </c>
       <c r="L48" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-4.5</v>
       </c>
       <c r="M48" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-4.5</v>
       </c>
       <c r="N48" s="23"/>
     </row>
@@ -5523,12 +5551,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A28:A39"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A6:A17"/>
-    <mergeCell ref="A18:A25"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -5539,6 +5561,12 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A28:A39"/>
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A6:A17"/>
+    <mergeCell ref="A18:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
put in hours worked for daniel
</commit_message>
<xml_diff>
--- a/documents/Burndown.xlsx
+++ b/documents/Burndown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Burndown" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -603,27 +603,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent1 2" xfId="1"/>
@@ -867,11 +868,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88637824"/>
-        <c:axId val="88639360"/>
+        <c:axId val="103438976"/>
+        <c:axId val="103498112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88637824"/>
+        <c:axId val="103438976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,7 +881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88639360"/>
+        <c:crossAx val="103498112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -888,7 +889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88639360"/>
+        <c:axId val="103498112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -899,7 +900,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88637824"/>
+        <c:crossAx val="103438976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1159,11 +1160,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88959616"/>
-        <c:axId val="88985984"/>
+        <c:axId val="106065920"/>
+        <c:axId val="106067456"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="88959616"/>
+        <c:axId val="106065920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1173,14 +1174,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88985984"/>
+        <c:crossAx val="106067456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="88985984"/>
+        <c:axId val="106067456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1191,13 +1192,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88959616"/>
+        <c:crossAx val="106065920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1287,31 +1289,31 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.5</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.5</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-4.5</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,11 +1416,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="90629248"/>
-        <c:axId val="90630784"/>
+        <c:axId val="106717184"/>
+        <c:axId val="106718720"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="90629248"/>
+        <c:axId val="106717184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,14 +1430,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90630784"/>
+        <c:crossAx val="106718720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="90630784"/>
+        <c:axId val="106718720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +1448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90629248"/>
+        <c:crossAx val="106717184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1864,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,13 +1983,16 @@
       </c>
       <c r="D5" s="4">
         <f>H4-E5</f>
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E5" s="3">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="F5" s="3">
+        <v>32</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="4">
         <v>125</v>
@@ -2004,7 +2009,10 @@
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="4">
+        <f>H5-E6</f>
+        <v>125</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
@@ -4076,8 +4084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4199,7 +4207,7 @@
       <c r="A6" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="77">
+      <c r="B6" s="75">
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -4252,7 +4260,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="63"/>
-      <c r="B7" s="78"/>
+      <c r="B7" s="76"/>
       <c r="C7" s="45" t="s">
         <v>16</v>
       </c>
@@ -4273,30 +4281,30 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="63"/>
-      <c r="B8" s="78"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="24">
         <v>2</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
       <c r="N8" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(E30:M30)</f>
+        <v>-42</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="63"/>
-      <c r="B9" s="79"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -4317,7 +4325,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="63"/>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -4370,7 +4378,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="63"/>
-      <c r="B11" s="81"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
@@ -4391,7 +4399,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="63"/>
-      <c r="B12" s="81"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
@@ -4412,7 +4420,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="63"/>
-      <c r="B13" s="81"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -4435,7 +4443,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="63"/>
-      <c r="B14" s="81"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="52" t="s">
         <v>33</v>
       </c>
@@ -4486,7 +4494,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="63"/>
-      <c r="B15" s="81"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="45" t="s">
         <v>16</v>
       </c>
@@ -4513,7 +4521,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="63"/>
-      <c r="B16" s="81"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
@@ -4536,7 +4544,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="63"/>
-      <c r="B17" s="81"/>
+      <c r="B17" s="79"/>
       <c r="C17" s="45" t="s">
         <v>18</v>
       </c>
@@ -4679,7 +4687,7 @@
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="63"/>
-      <c r="B22" s="75"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="49" t="s">
         <v>31</v>
       </c>
@@ -4730,7 +4738,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="63"/>
-      <c r="B23" s="75"/>
+      <c r="B23" s="80"/>
       <c r="C23" s="45" t="s">
         <v>16</v>
       </c>
@@ -4751,7 +4759,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="63"/>
-      <c r="B24" s="75"/>
+      <c r="B24" s="80"/>
       <c r="C24" s="45" t="s">
         <v>17</v>
       </c>
@@ -4772,7 +4780,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="64"/>
-      <c r="B25" s="76"/>
+      <c r="B25" s="81"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -4853,7 +4861,7 @@
       <c r="A28" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="77">
+      <c r="B28" s="75">
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -4865,45 +4873,45 @@
       </c>
       <c r="E28" s="16">
         <f t="shared" ref="E28:M28" si="7">SUM(E29:E31)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="G28" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H28" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I28" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="J28" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="K28" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="L28" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="M28" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="N28" s="23"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="63"/>
-      <c r="B29" s="78"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="45" t="s">
         <v>16</v>
       </c>
@@ -4924,28 +4932,46 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="63"/>
-      <c r="B30" s="78"/>
+      <c r="B30" s="76"/>
       <c r="C30" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="57">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
+        <f>D8</f>
+        <v>2</v>
+      </c>
+      <c r="E30" s="31">
+        <v>2</v>
+      </c>
+      <c r="F30" s="31">
+        <v>-2</v>
+      </c>
+      <c r="G30" s="31">
+        <v>-2</v>
+      </c>
+      <c r="H30" s="31">
+        <v>-2</v>
+      </c>
+      <c r="I30" s="32">
+        <v>-6</v>
+      </c>
+      <c r="J30" s="32">
+        <v>-8</v>
+      </c>
+      <c r="K30" s="32">
+        <v>-8</v>
+      </c>
+      <c r="L30" s="32">
+        <v>-8</v>
+      </c>
+      <c r="M30" s="32">
+        <v>-8</v>
+      </c>
       <c r="N30" s="24"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="63"/>
-      <c r="B31" s="79"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="46" t="s">
         <v>18</v>
       </c>
@@ -4966,7 +4992,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="63"/>
-      <c r="B32" s="80" t="s">
+      <c r="B32" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="47" t="s">
@@ -4978,23 +5004,23 @@
       </c>
       <c r="E32" s="16">
         <f t="shared" ref="E32:M32" si="9">SUM(E33:E35)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="16">
         <f t="shared" si="9"/>
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="J32" s="16">
         <f t="shared" si="9"/>
@@ -5016,7 +5042,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="63"/>
-      <c r="B33" s="81"/>
+      <c r="B33" s="79"/>
       <c r="C33" s="45" t="s">
         <v>16</v>
       </c>
@@ -5040,22 +5066,22 @@
         <v>-0.5</v>
       </c>
       <c r="J33" s="32">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="K33" s="32">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="L33" s="32">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="M33" s="32">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="N33" s="24"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="63"/>
-      <c r="B34" s="81"/>
+      <c r="B34" s="79"/>
       <c r="C34" s="45" t="s">
         <v>17</v>
       </c>
@@ -5076,7 +5102,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="63"/>
-      <c r="B35" s="81"/>
+      <c r="B35" s="79"/>
       <c r="C35" s="46" t="s">
         <v>18</v>
       </c>
@@ -5084,20 +5110,38 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="34"/>
+      <c r="E35" s="33">
+        <v>1</v>
+      </c>
+      <c r="F35" s="33">
+        <v>1</v>
+      </c>
+      <c r="G35" s="33">
+        <v>1</v>
+      </c>
+      <c r="H35" s="33">
+        <v>1</v>
+      </c>
+      <c r="I35" s="33">
+        <v>1</v>
+      </c>
+      <c r="J35" s="33">
+        <v>1</v>
+      </c>
+      <c r="K35" s="33">
+        <v>1</v>
+      </c>
+      <c r="L35" s="33">
+        <v>1</v>
+      </c>
+      <c r="M35" s="33">
+        <v>1</v>
+      </c>
       <c r="N35" s="24"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="63"/>
-      <c r="B36" s="81"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="52" t="s">
         <v>33</v>
       </c>
@@ -5107,45 +5151,45 @@
       </c>
       <c r="E36" s="16">
         <f t="shared" ref="E36:M36" si="10">SUM(E37:E39)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F36" s="16">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G36" s="16">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H36" s="16">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I36" s="16">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J36" s="16">
         <f t="shared" si="10"/>
-        <v>1.5</v>
+        <v>-2</v>
       </c>
       <c r="K36" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L36" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M36" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="N36" s="23"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="63"/>
-      <c r="B37" s="81"/>
+      <c r="B37" s="79"/>
       <c r="C37" s="45" t="s">
         <v>16</v>
       </c>
@@ -5171,14 +5215,20 @@
       <c r="J37" s="32">
         <v>1.5</v>
       </c>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
+      <c r="K37" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="L37" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="M37" s="32">
+        <v>1.5</v>
+      </c>
       <c r="N37" s="24"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="63"/>
-      <c r="B38" s="81"/>
+      <c r="B38" s="79"/>
       <c r="C38" s="45" t="s">
         <v>17</v>
       </c>
@@ -5186,20 +5236,38 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
+      <c r="E38" s="31">
+        <v>3</v>
+      </c>
+      <c r="F38" s="31">
+        <v>3</v>
+      </c>
+      <c r="G38" s="31">
+        <v>3</v>
+      </c>
+      <c r="H38" s="31">
+        <v>3</v>
+      </c>
+      <c r="I38" s="31">
+        <v>3</v>
+      </c>
+      <c r="J38" s="32">
+        <v>-3.5</v>
+      </c>
+      <c r="K38" s="32">
+        <v>-3.5</v>
+      </c>
+      <c r="L38" s="32">
+        <v>-3.5</v>
+      </c>
+      <c r="M38" s="32">
+        <v>-3.5</v>
+      </c>
       <c r="N38" s="24"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="63"/>
-      <c r="B39" s="81"/>
+      <c r="B39" s="79"/>
       <c r="C39" s="45" t="s">
         <v>18</v>
       </c>
@@ -5232,39 +5300,39 @@
       </c>
       <c r="E40" s="16">
         <f t="shared" ref="E40:M40" si="11">SUM(E41:E43)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F40" s="16">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G40" s="16">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H40" s="16">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I40" s="16">
         <f t="shared" si="11"/>
-        <v>-3.5</v>
+        <v>-1.5</v>
       </c>
       <c r="J40" s="16">
         <f t="shared" si="11"/>
-        <v>-3.5</v>
+        <v>-6.5</v>
       </c>
       <c r="K40" s="16">
         <f t="shared" si="11"/>
-        <v>-3.5</v>
+        <v>-6.5</v>
       </c>
       <c r="L40" s="16">
         <f t="shared" si="11"/>
-        <v>-3.5</v>
+        <v>-6.5</v>
       </c>
       <c r="M40" s="16">
         <f t="shared" si="11"/>
-        <v>-3.5</v>
+        <v>-6.5</v>
       </c>
       <c r="N40" s="23"/>
     </row>
@@ -5317,15 +5385,33 @@
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
+      <c r="E42" s="31">
+        <v>2</v>
+      </c>
+      <c r="F42" s="31">
+        <v>2</v>
+      </c>
+      <c r="G42" s="31">
+        <v>2</v>
+      </c>
+      <c r="H42" s="31">
+        <v>2</v>
+      </c>
+      <c r="I42" s="31">
+        <v>2</v>
+      </c>
+      <c r="J42" s="32">
+        <v>-3</v>
+      </c>
+      <c r="K42" s="32">
+        <v>-3</v>
+      </c>
+      <c r="L42" s="32">
+        <v>-3</v>
+      </c>
+      <c r="M42" s="32">
+        <v>-3</v>
+      </c>
       <c r="N42" s="24"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -5351,7 +5437,7 @@
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="63"/>
-      <c r="B44" s="75"/>
+      <c r="B44" s="80"/>
       <c r="C44" s="49" t="s">
         <v>31</v>
       </c>
@@ -5361,45 +5447,45 @@
       </c>
       <c r="E44" s="21">
         <f t="shared" ref="E44:M44" si="12">SUM(E45:E47)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="21">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="21">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="21">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="21">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="21">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="K44" s="21">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="L44" s="21">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="M44" s="21">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="N44" s="23"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="63"/>
-      <c r="B45" s="75"/>
+      <c r="B45" s="80"/>
       <c r="C45" s="45" t="s">
         <v>16</v>
       </c>
@@ -5420,7 +5506,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="63"/>
-      <c r="B46" s="75"/>
+      <c r="B46" s="80"/>
       <c r="C46" s="45" t="s">
         <v>17</v>
       </c>
@@ -5428,20 +5514,38 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
+      <c r="E46" s="31">
+        <v>0</v>
+      </c>
+      <c r="F46" s="31">
+        <v>0</v>
+      </c>
+      <c r="G46" s="31">
+        <v>0</v>
+      </c>
+      <c r="H46" s="31">
+        <v>0</v>
+      </c>
+      <c r="I46" s="31">
+        <v>0</v>
+      </c>
+      <c r="J46" s="31">
+        <v>-1.5</v>
+      </c>
+      <c r="K46" s="31">
+        <v>-1.5</v>
+      </c>
+      <c r="L46" s="31">
+        <v>-1.5</v>
+      </c>
+      <c r="M46" s="31">
+        <v>-1.5</v>
+      </c>
       <c r="N46" s="24"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="64"/>
-      <c r="B47" s="76"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
@@ -5449,15 +5553,33 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="34"/>
-      <c r="L47" s="34"/>
-      <c r="M47" s="34"/>
+      <c r="E47" s="33">
+        <v>1</v>
+      </c>
+      <c r="F47" s="33">
+        <v>1</v>
+      </c>
+      <c r="G47" s="33">
+        <v>1</v>
+      </c>
+      <c r="H47" s="33">
+        <v>1</v>
+      </c>
+      <c r="I47" s="33">
+        <v>1</v>
+      </c>
+      <c r="J47" s="33">
+        <v>1</v>
+      </c>
+      <c r="K47" s="33">
+        <v>1</v>
+      </c>
+      <c r="L47" s="33">
+        <v>1</v>
+      </c>
+      <c r="M47" s="33">
+        <v>1</v>
+      </c>
       <c r="N47" s="24"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -5471,39 +5593,39 @@
       </c>
       <c r="E48" s="2">
         <f t="shared" ref="E48:M48" si="13">SUM(E28,E32,E36,E40,E44)</f>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F48" s="2">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="13"/>
-        <v>-3</v>
+        <v>-18</v>
       </c>
       <c r="K48" s="2">
         <f t="shared" si="13"/>
-        <v>-4.5</v>
+        <v>-18</v>
       </c>
       <c r="L48" s="2">
         <f t="shared" si="13"/>
-        <v>-4.5</v>
+        <v>-18</v>
       </c>
       <c r="M48" s="2">
         <f t="shared" si="13"/>
-        <v>-4.5</v>
+        <v>-18</v>
       </c>
       <c r="N48" s="23"/>
     </row>
@@ -5551,6 +5673,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A28:A39"/>
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A6:A17"/>
+    <mergeCell ref="A18:A25"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -5561,12 +5689,6 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A28:A39"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A6:A17"/>
-    <mergeCell ref="A18:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>